<commit_message>
correction gestion admin(formulaire inscription admin) + plan test + correction controller admin pour suppression et mise à jour + ajout middle admin + ajout route admin + amélioration balise sémantique + css visibilité + ajout adminView + amélioration bouton upload
</commit_message>
<xml_diff>
--- a/P7_ZHANG_plan_test.xlsx
+++ b/P7_ZHANG_plan_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33613\Documents\Formation DEV WEB\007_projet_7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33613\Documents\Formation DEV WEB\007_projet_7\Groupmania_Jing_ZHANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A83C35-8E56-407F-8E4F-39892E0D3695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B688BF-3269-4178-81D3-6040AE3D5833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,15 +58,6 @@
     </r>
   </si>
   <si>
-    <t>- Remplir l'email en respectant le format
-- Remplir le mot de passe en respectant le format
-- Cliquer sur le lien "inscrivez-vous"</t>
-  </si>
-  <si>
-    <t>- Remplir les champs de formulaire en respectant les formats concernés
-- Cliquer sur le lien "se connecter"</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Une </t>
     </r>
@@ -76,171 +67,38 @@
         <color theme="4"/>
         <rFont val="Montserrat"/>
       </rPr>
-      <t xml:space="preserve">page </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>"inscription"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
+      <t>page "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>créer un post</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <rFont val="Montserrat"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>montrant de manière dynamique 2 possibilités de connexion (inscription + connexion)</t>
-    </r>
-  </si>
-  <si>
-    <t>-Pour l'inscription des comptes:
- 1) en cas de réussite: se diriger vers la page liste des posts.
- 2) en cas d'échec: 
--&gt;le bouton "se connecter" est grisé
--&gt;affichage de message d'invalidation des champs 
--&gt;affichage de message d'erreur de connexion
-- Lors du click sur le lien "se connecter", se diriger vers la page "se connecter"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Une </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>page "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>créer un post</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>- quand pas de publication : cliquer sur le lien "créer un post" de la barre de navigation
-- quand il y a déjà des posts : montrant de manière  dynaminque les posts des utilisateurs
-- cliquer les 4 liens (créer un post, mon profile, deconnexion, listes des posts) dans la barre de navigation</t>
   </si>
   <si>
     <t>- Remplir les champs de formulaire (title &amp; description)
 - Choisir une image et l'uploader
 - Valider le formulaire
 - Cliquer les liens de la barre de navigation</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Une </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>page "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>liste des posts</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>-Pour la validation de formulaire:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
- 1) en cas de réussite: se diriger vers la page liste des posts.
-2) en cas de réussite d'uploder l'image: affichage message de confirmation
- 2) en cas d'échec: 
--&gt;le bouton "se connecter" est grisé
--&gt;affichage de message d'invalidation des champs 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>- Pour les liens de la barre de navigation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">
-1) si c'est sur "liste des posts ", se diriger vers la page "liste des posts"
-2) si c'est sur "mon profil", se diriger vers la page "mon profil"
-3) si c'est sur "déconexion", se déconnecter et se diriger vers la page de connexion</t>
-    </r>
   </si>
   <si>
     <t>- Modifer les champs de formulaire (title &amp; description)
@@ -248,6 +106,319 @@
 - Valider le formulaire
 - Supprimer le compte
 - Cliquer les liens de la barre de navigation</t>
+  </si>
+  <si>
+    <t>- Modifer les champs de formulaire (title &amp; description)
+- Choisir une image et l'uploader
+- Valider le formulaire
+- Cliquer les liens de la barre de navigation</t>
+  </si>
+  <si>
+    <r>
+      <t>Une</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> "mon profil"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Une </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> "modifier un post"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Une </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>"Login"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Une </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">page </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>"sign-up"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Une </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>page</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> "sign-up Admin" </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>pour administrateur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Pour </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>login</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>:
+1) si OK =&gt; se diriger vers la page liste des posts.
+2) si KO
+-&gt;le bouton "se connecter" est grisé
+-&gt;affichage de message d'invalidation des champs 
+-&gt;affichage de message d'erreur de connexion
+3) si déjà connecté, se diriger directement sur la liste des posts
+- Lors du click du lien "inscrivez-vous", se diriger vers la page "sign-up"</t>
+    </r>
+  </si>
+  <si>
+    <t>- Remplir les champs en respectant les formats
+- Cliquer sur le lien "inscrivez-vous"pour s'inscrire</t>
+  </si>
+  <si>
+    <t>- Remplir les champs en respectant les formats
+- Cliquer sur le lien "se connecter" pour se connecter</t>
+  </si>
+  <si>
+    <t>-Pour signup:
+ 1) si OK =&gt; se diriger vers la page liste des posts.
+ 2) si KO
+-&gt;le bouton "se connecter" est grisé
+-&gt;affichage de message d'invalidation des champs 
+-&gt;affichage de message d'erreur de connexion
+- Lors du click sur le lien "se connecter", se diriger vers la page "se connecter"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Remplir les champs en respectant les formats concernés </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 1) si OK 
+-&gt; se diriger vers la page liste des posts 
+-&gt; la personne qui se connecte est administrateur
+ 2) si KO
+-&gt;le bouton "se connecter" est grisé
+-&gt;affichage de message d'invalidation des champs 
+-&gt;affichage de message d'erreur de connexion
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Une </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>page "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>liste des posts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="4"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> montrant le contenu des posts des utilisateurs</t>
+    </r>
+  </si>
+  <si>
+    <t>=&gt; quand l'utilisateur est administrateur / créateur des posts : 
+- "supprimer un post" 
+- "modifier un post" 
+- "supprimer un commentaire"
+-  "envoyer un commentaire" 
+=&gt;cliquer les 4 liens (créer un post, mon profile, deconnexion, listes des posts) dans la barre de navigation</t>
+  </si>
+  <si>
+    <t>=&gt;affichage de tous les posts du plus récent au moins récent (titre, description, image, date, photo)
+=&gt; afichage de tous les commentaires du plus récent au moins récent
+=&gt; Un champ pour écrire d'un commentaire: 
+=&gt; Quand c'est le créateur des posts / admin : 
+- Les boutons "modifier le post / supprimer le post / supprimer un commentaire" doivent apparaître 
+=&gt; modifer le post lors du click sur le bouton "modifier"
+=&gt; supprimer le postlors du click sur le bouton "supprimer"
+=&gt; supprimer un commentaire lors du click sur le bouton "supprimer"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>-Pour la validation de formulaire:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+ 1) Si OK: 
+=&gt; se diriger vers la page liste des posts.
+=&gt; uploader l'image
+ 2) SI KO
+-&gt;le bouton "se connecter" est grisé
+-&gt;affichage de message d'erreur des champs 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>- Pour les liens de la barre de navigation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve">
+1) pour les liens, se diriger vers les pages concernées
+2) si "déconexion", se déconnecter et se diriger vers la page de connexion</t>
+    </r>
   </si>
   <si>
     <r>
@@ -309,16 +480,9 @@
         <rFont val="Montserrat"/>
       </rPr>
       <t xml:space="preserve">
-1) si c'est sur "liste des posts ", se diriger vers la page "liste des posts"
-2) si c'est sur "créer un post", se diriger vers la page "créer un post"
-3) si c'est sur "déconnexion", se déconnecter et se diriger vers la page de connexion</t>
-    </r>
-  </si>
-  <si>
-    <t>- Modifer les champs de formulaire (title &amp; description)
-- Choisir une image et l'uploader
-- Valider le formulaire
-- Cliquer les liens de la barre de navigation</t>
+1) pour les liens, se diriger vers les pages concernées
+2) si "déconexion", se déconnecter et se diriger vers la page de connexion</t>
+    </r>
   </si>
   <si>
     <r>
@@ -360,164 +524,16 @@
         <rFont val="Montserrat"/>
       </rPr>
       <t xml:space="preserve">
-1) si c'est sur "liste des posts ", se diriger vers la page "liste des posts"
-2) si c'est sur "créer un post", se diriger vers la page "créer un post"
-3) si c'est sur "déconnexion", se déconnecter et se diriger vers la page de connexion</t>
-    </r>
-  </si>
-  <si>
-    <t>- Cliquer sur le bouton "transformer en admin"
-- Cliquer sur le lien "retour sur la liste des posts"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- L'utilisateur est transformé en Admin s'il n'est pas
-- Le bouton est grisé une fois que la transformation est faite avec un message d'indication
-- Lors de reconnexion, si l'utilisateur est déjà Admin, un message indique le rôle de l'utilisateur
-- Un message indique le rôle de l'utilisateur dans "mon profil"
-- L'utilisateur peut retourner sur la liste des posts </t>
-  </si>
-  <si>
-    <t>-Pour la connexion des comptes:
- 1) en cas de réussite: se diriger vers la page liste des posts.
- 2) en cas d'échec: 
--&gt;le bouton "se connecter" est grisé
--&gt;affichage de message d'invalidation des champs 
--&gt;affichage de message d'erreur de connexion
-3) si l'utilisateur est déjà connecté,  lors de l'actualistion de page, se diriger directement sur la liste des posts
-- Lors du clique sur le lien "inscrivez-vous", se diriger vers la page "inscription"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Une </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">page </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>"se connecter"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> montrant de manière dynamique la possibilité de connexion "signup" si l'utilisateur n'a pas de compte</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Une</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>page</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> "mon profil"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Une </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>page</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> "transformer en admin"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Une </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>page</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="4"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve"> "modifier un post"</t>
-    </r>
-  </si>
-  <si>
-    <t>- L'affichage de tous les posts du plus récent au moins récent (titre, description, image, date, photo)
-- L'affichage de tous les commentaires du plus récent au moins récent
-- Un champ pour écrire d'un commentaire
-- Les boutons "modifier / supprimer le post" doivent apparaitre si c'est le créateur des posts/administrateur
-- Le bouton de "supprimer un commentaire" doit appraitre si c'est le créateur des posts/administrateur</t>
+1) pour les liens, se diriger vers les pages concernées
+2) si "déconexion", se déconnecter et se diriger vers la page de connexion</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -562,6 +578,12 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <u/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Montserrat"/>
@@ -974,7 +996,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1002,18 +1024,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="190.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="214.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>4</v>
@@ -1024,81 +1046,81 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:5" ht="174" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="252" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="272.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="315" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="278.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" s="8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>6</v>
+    <row r="7" spans="1:5" ht="313.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>4</v>
@@ -1109,13 +1131,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
ajout schema MCD + modif plan test + amélioration listOfComments
</commit_message>
<xml_diff>
--- a/P7_ZHANG_plan_test.xlsx
+++ b/P7_ZHANG_plan_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33613\Documents\Formation DEV WEB\007_projet_7\Groupmania_Jing_ZHANG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B688BF-3269-4178-81D3-6040AE3D5833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705CD6EF-511D-4C64-B1E3-9E90870B1E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -995,8 +995,8 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
     </row>
     <row r="6" spans="1:5" ht="278.39999999999998" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>5</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="7" spans="1:5" ht="313.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>9</v>

</xml_diff>